<commit_message>
Testcases commit-Landing test case, Testcases title change
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -38,9 +38,6 @@
     <t>Tap on "CONTINUE WITH FACEBOOK" button</t>
   </si>
   <si>
-    <t>Verify Home page</t>
-  </si>
-  <si>
     <t>Expected Result</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>Quit the app</t>
+  </si>
+  <si>
+    <t>Verify Landing page</t>
   </si>
 </sst>
 </file>
@@ -116,23 +116,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,13 +445,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -462,42 +462,42 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>6</v>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="9"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>